<commit_message>
Atualização automática de CACEQUI.xlsx
</commit_message>
<xml_diff>
--- a/CACEQUI.xlsx
+++ b/CACEQUI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81E7DFE9-45E6-42FE-A996-BB14C98BCE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79201B49-F4CC-4DE1-9537-B02DB9A0AFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1115,7 +1102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1175,36 +1162,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1243,14 +1206,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1303,7 +1261,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{D22C6D22-7203-4F81-8C5B-019651144694}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{8F82E762-2577-40E7-A76F-771701618D8E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1333,10 +1291,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11B2AF8C-1A46-4391-843E-5AF0F9CCE749}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB9BE9E-7243-468F-B2E2-AD4CB7562C38}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1374,7 +1332,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FCDF059-1C7B-4AB9-A5A6-221D58456644}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54D2091A-D17F-4B54-9913-743FCA5B887D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1395,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FE947F1-8646-44B7-82B9-DFB826EFA8CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E0DEB9-0C6B-43F7-9331-F218DEF62EAF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,7 +1414,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA4645CE-0378-290B-99D6-5E445D30C6B7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0714ED52-30A9-4CFA-D206-4946D0ED6D21}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1505,7 +1463,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{599A5BA8-6ACC-42C4-E7BE-93FE9DB53A7D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D0BBA2-6309-88A9-E21E-1BDB9B6340DC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1524,7 +1482,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91E2D5D-FDD0-D527-2D26-061D8255062C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7A1E423-7270-3302-C1FA-3CF9738FEFD9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1555,7 +1513,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8672D5B9-4FC7-A368-41D1-B539C7D5FDA5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED2F7E92-674A-E50F-5466-C42F03A789BD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1586,7 +1544,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219FE8EC-74DF-3093-735C-FF7F35CF9C53}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9229361-6C7D-BBC5-F751-30217EC7664F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1629,7 +1587,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973225D8-2C70-4F30-A279-AB88BD7CD754}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4EF0AF-4E3E-4A61-A4AF-092DC7D114A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1667,7 +1625,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76A86426-43BE-4585-A268-302146BBCF7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB59F345-97D7-4BE7-B751-3E3F2E3532CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1710,7 +1668,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7942C71-22AD-4618-A24A-D3A8AAFA377E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD30B7A2-43CE-413F-8296-605032DC20C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,7 +1981,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384C28D-91CB-4DBC-8317-FAB7BE749E2B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B584ADA-342C-4F6E-95A2-21367978358D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2035,98 +1993,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5362,19 +5320,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5397,46 +5355,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5454,16 +5412,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5497,7 +5455,7 @@
       <c r="J1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>286</v>
       </c>
     </row>
@@ -5511,10 +5469,10 @@
       <c r="C2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>879.9</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>87.99</v>
       </c>
       <c r="F2" s="2">
@@ -5532,7 +5490,7 @@
       <c r="J2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>18637</v>
       </c>
     </row>
@@ -5546,10 +5504,10 @@
       <c r="C3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="21">
         <v>36</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>3.6</v>
       </c>
       <c r="F3" s="2">
@@ -5567,7 +5525,7 @@
       <c r="J3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>8860</v>
       </c>
     </row>
@@ -5592,54 +5550,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>308</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>309</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5650,43 +5609,43 @@
       <c r="B2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <v>45170</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="27">
         <v>830</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>2717</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>287</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>313</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>313</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>315</v>
       </c>
     </row>
@@ -5717,25 +5676,24 @@
       <c r="B1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>317</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="35">
         <v>18</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" s="38">
-        <v>18</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>1.190318740907287E-3</v>
       </c>
     </row>

</xml_diff>